<commit_message>
Stabilised the Excel with Corner Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/XLSX/empty_file.xlsx
+++ b/src/test/resources/XLSX/empty_file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/docflex/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/docflex/IdeaProjects/UnifiedReporter/src/test/resources/XLSX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C756DC5-2ACF-E841-A6E1-32442B212314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29728A72-BCC1-754C-A677-8AB9D0AAECF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{B77BA239-30B6-A748-8FA6-7454C8ABC2AF}"/>
   </bookViews>
@@ -32,10 +32,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,9 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00191AA0-D552-114B-A1D5-94FBE662DC59}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>